<commit_message>
Added comments to LetterGen -DW
Added comments for easier understanding of what's being executed in the main program.
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devon\Desktop\ChristmasCardProgram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C512A2-979F-4E54-89DE-96332A1AEAA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67F5DD1-0EC9-48BC-B3E0-731DFF83B4E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{65E6B7E1-27B2-460A-9B06-41F6A047FB4D}"/>
   </bookViews>
@@ -431,15 +431,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92546D7B-288A-4707-9227-08A5E4B7D352}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>